<commit_message>
update front style + Mela B3 Serum
</commit_message>
<xml_diff>
--- a/database/tables/lrp.xlsx
+++ b/database/tables/lrp.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$K$133</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$K$132</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="431">
   <si>
     <t xml:space="preserve">EAN</t>
   </si>
@@ -2164,11 +2164,22 @@
     <t xml:space="preserve">MELA B3 SERUM</t>
   </si>
   <si>
-    <t xml:space="preserve">La Roche Posay es una marca que ofrece una variedad de productos para el cuidado de la piel facial. Si buscas protegerla y mantenerla en forma, esta puede ser una buena opción.
-Cuidados para combatir manchas
-Los productos antimanchas ayudan a prevenir y reducir marcas en el rostro, como así también lograr un aspecto uniforme y sin hiperpigmentación. Además, es importante proteger la piel de los rayos dañinos del sol para complementar el cuidado.
-Libre de parabenos
-Los productos libres de parabenos son una buena opción para el cuidado de pieles sensibles o para quienes eligen productos sin conservantes artificiales.</t>
+    <t xml:space="preserve">Serum antiedad intensivo antimanchas, antireaparición. Testeado clínicamente, corrige las manchas oscuras, incluso las más persistentes. Testeado clínicamente en todos los tonos de piel y todos los tipos de manchas oscuras, incluidas las manchas de la edad, las manchas solares, las marcas pigmentadas post-acné y post-cicatrización. Reduce la hiperpigmentación, iguala el tono de la piel y las marcas de acné. Alta eficacia garantizando la tolerancia incluso en pieles sensibles. No comedogénico. ¿Conocías Pure Niacinamida 10? Descubre su evolución a Mela B3 Serum, la nueva revolución despigmentante. Una fórmula mejorada con mayor eficacia. Conservando el poder del 10% de Niacinamida, esta nueva fórmula incorpora un complejo de activos potentes, incluyendo Melasyl, el nuevo activo multipatentado para luchar contra la hiperpigmentación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contiene Melasyl, inovación en hiperpigmentación. Melasyl es una molécula revolucionaria multipatentada. Contiene Niacinamida, una forma de vitamina B3. La niacinamida es una vitamina soluble en agua. Se utiliza a menudo en dermocosmética y se la conoce por su capacidad para calmar la piel, reforzar la barrera cutánea y corregir las manchas. Contiene agua termal, la cual trata las irritaciones de la piel y las calma profundamente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrige las manchas en el rostro, incluso las persistentes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unifica el tono de la piel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eficacia anti-reaparición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantidad de 2 a 3 gotas. Durante la mañana y/o la noche. Aplicar en el rostro, cuello, escote y manos. Aplicar después de la limpieza. Puede usarse solo o antes de una crema hidratante. </t>
   </si>
 </sst>
 </file>
@@ -2659,208 +2670,212 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2868,151 +2883,151 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3020,15 +3035,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3337,2916 +3352,2915 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B130" activeCellId="0" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="75.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="75.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="16.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="12" t="n">
         <v>7790033283244</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="12" t="n">
         <v>7790033283237</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="12" t="n">
         <v>7790033283268</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="12" t="n">
         <v>7790033283251</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+      <c r="A8" s="16" t="n">
         <v>30162457</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="17" t="n">
         <v>50</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="14" t="n">
         <v>250</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="n">
+      <c r="A10" s="22" t="n">
         <v>3337875588560</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+      <c r="A11" s="22" t="n">
         <v>3337875549530</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>75</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="21" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="n">
+      <c r="A12" s="23" t="n">
         <v>30159983</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
+      <c r="A13" s="23" t="n">
         <v>30157439</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="n">
+      <c r="A14" s="22" t="n">
         <v>3433422408616</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="7" t="n">
         <v>125</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
+      <c r="A17" s="25" t="n">
         <v>3337875706674</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
+      <c r="A18" s="25" t="n">
         <v>3337875706681</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
+      <c r="A19" s="25" t="n">
         <v>3337875696838</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="6" t="n">
+      <c r="D19" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
+      <c r="A20" s="25" t="n">
         <v>3337875728188</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="D20" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="6" t="n">
+      <c r="D21" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D22" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="n">
+      <c r="A23" s="26" t="n">
         <v>3337875763790</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="28" t="n">
+      <c r="D23" s="29" t="n">
         <v>200</v>
       </c>
-      <c r="E23" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="29" t="s">
+      <c r="E23" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I23" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="32" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D24" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="8" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="n">
+      <c r="A25" s="25" t="n">
         <v>3433422404533</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D25" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="8" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24" t="n">
+      <c r="A27" s="25" t="n">
         <v>3337875586269</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="17" t="s">
+      <c r="E27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="J27" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="K27" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="6" t="n">
+      <c r="D28" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="17" t="s">
+      <c r="E28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24" t="n">
+      <c r="A29" s="25" t="n">
         <v>3337872413018</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="6" t="n">
+      <c r="D29" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="17" t="s">
+      <c r="E29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="n">
+      <c r="A30" s="25" t="n">
         <v>3337875517300</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="6" t="n">
+      <c r="D30" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="17" t="s">
+      <c r="E30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K30" s="8" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D31" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="32" t="s">
+      <c r="E31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D32" s="7" t="n">
         <v>7.5</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="32" t="s">
+      <c r="E32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K32" s="8" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="n">
+      <c r="A33" s="25" t="n">
         <v>3337875632676</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D33" s="7" t="n">
         <v>4.5</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="6" t="s">
+      <c r="E33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K33" s="8" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="n">
+      <c r="A34" s="25" t="n">
         <v>3337875632690</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D34" s="6" t="n">
+      <c r="D34" s="7" t="n">
         <v>4.5</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="6" t="s">
+      <c r="E34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="K34" s="7" t="s">
+      <c r="K34" s="8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D35" s="7" t="n">
         <v>125</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24" t="n">
+      <c r="A37" s="25" t="n">
         <v>3337875549486</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D37" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="24" t="n">
+      <c r="A38" s="25" t="n">
         <v>3337875598071</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="D38" s="6" t="n">
+      <c r="D38" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="D39" s="6" t="n">
+      <c r="D39" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="24" t="n">
+      <c r="A40" s="25" t="n">
         <v>7899706149211</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="D40" s="6" t="n">
+      <c r="D40" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="D41" s="6" t="n">
+      <c r="D41" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="D42" s="6" t="n">
+      <c r="D42" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="24" t="n">
+      <c r="A43" s="25" t="n">
         <v>3337872420207</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D43" s="6" t="n">
+      <c r="D43" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24" t="n">
+      <c r="A44" s="25" t="n">
         <v>3337875613491</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="D44" s="6" t="n">
+      <c r="D44" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15" t="n">
+      <c r="A45" s="16" t="n">
         <v>3337875518451</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="D45" s="6" t="n">
+      <c r="D45" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15" t="n">
+      <c r="A46" s="16" t="n">
         <v>3337875518598</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="D46" s="6" t="n">
+      <c r="D46" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="34" t="n">
+      <c r="A47" s="35" t="n">
         <v>3337872412776</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="D47" s="36" t="n">
+      <c r="D47" s="37" t="n">
         <v>50</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E47" s="38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="38" t="n">
+      <c r="A48" s="39" t="n">
         <v>3337875518628</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="D48" s="40" t="n">
+      <c r="D48" s="41" t="n">
         <v>100</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="38" t="n">
+      <c r="A49" s="39" t="n">
         <v>3337875722827</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="D49" s="40" t="n">
+      <c r="D49" s="41" t="n">
         <v>30</v>
       </c>
-      <c r="E49" s="41" t="s">
+      <c r="E49" s="42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="D50" s="6" t="n">
+      <c r="D50" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="D51" s="6" t="n">
+      <c r="D51" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="24" t="n">
+      <c r="A52" s="25" t="n">
         <v>3337872412042</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="D52" s="6" t="n">
+      <c r="D52" s="7" t="n">
         <v>9.5</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24" t="n">
+      <c r="A53" s="25" t="n">
         <v>3337872412059</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="D53" s="6" t="n">
+      <c r="D53" s="7" t="n">
         <v>9.5</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="D54" s="6" t="n">
+      <c r="D54" s="7" t="n">
         <v>9.5</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="C55" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="D55" s="6" t="n">
+      <c r="D55" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="D56" s="6" t="n">
+      <c r="D56" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="D57" s="6" t="n">
+      <c r="D57" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="D58" s="6" t="n">
+      <c r="D58" s="7" t="n">
         <v>2.6</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="25" t="s">
         <v>272</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="D59" s="6" t="n">
+      <c r="D59" s="7" t="n">
         <v>2.6</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="C60" s="23" t="s">
+      <c r="C60" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="D60" s="6" t="n">
+      <c r="D60" s="7" t="n">
         <v>2.6</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="D61" s="6" t="n">
+      <c r="D61" s="7" t="n">
         <v>2.6</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24" t="n">
+      <c r="A62" s="25" t="n">
         <v>3337875678667</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="C62" s="43" t="s">
+      <c r="C62" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="D62" s="6" t="n">
+      <c r="D62" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="24" t="n">
+      <c r="A63" s="25" t="n">
         <v>3337875678636</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="D63" s="6" t="n">
+      <c r="D63" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="D64" s="6" t="n">
+      <c r="D64" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="25" t="s">
         <v>287</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="D65" s="6" t="n">
+      <c r="D65" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15" t="n">
+      <c r="A66" s="16" t="n">
         <v>3337875528092</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C66" s="44" t="s">
+      <c r="C66" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="D66" s="16" t="n">
+      <c r="D66" s="17" t="n">
         <v>200</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15" t="n">
+      <c r="A67" s="16" t="n">
         <v>3337875528108</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C67" s="44" t="s">
+      <c r="C67" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="D67" s="6" t="n">
+      <c r="D67" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="D68" s="10" t="n">
+      <c r="D68" s="11" t="n">
         <v>195</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="45" t="n">
+      <c r="A69" s="46" t="n">
         <v>3337875528146</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C69" s="44" t="s">
+      <c r="C69" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="D69" s="46" t="n">
+      <c r="D69" s="47" t="n">
         <v>100</v>
       </c>
-      <c r="E69" s="47" t="s">
+      <c r="E69" s="48" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="45" t="n">
+      <c r="A70" s="46" t="n">
         <v>3337875725897</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C70" s="47" t="s">
+      <c r="C70" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="D70" s="46" t="n">
+      <c r="D70" s="47" t="n">
         <v>400</v>
       </c>
-      <c r="E70" s="47" t="s">
+      <c r="E70" s="48" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="45" t="n">
+      <c r="A71" s="46" t="n">
         <v>3337875725910</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C71" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="D71" s="46" t="n">
+      <c r="D71" s="47" t="n">
         <v>200</v>
       </c>
-      <c r="E71" s="47" t="s">
+      <c r="E71" s="48" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24" t="n">
+      <c r="A72" s="25" t="n">
         <v>3337872414053</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="C72" s="23" t="s">
+      <c r="C72" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="D72" s="6" t="n">
+      <c r="D72" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="15" t="n">
+      <c r="A73" s="16" t="n">
         <v>3337875660570</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="C73" s="43" t="s">
+      <c r="C73" s="44" t="s">
         <v>303</v>
       </c>
-      <c r="D73" s="6" t="n">
+      <c r="D73" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="24" t="n">
+      <c r="A74" s="25" t="n">
         <v>7790033284203</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C74" s="48" t="s">
+      <c r="C74" s="49" t="s">
         <v>305</v>
       </c>
-      <c r="D74" s="49" t="n">
+      <c r="D74" s="50" t="n">
         <v>50</v>
       </c>
-      <c r="E74" s="50" t="s">
+      <c r="E74" s="51" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="24" t="n">
+      <c r="A75" s="25" t="n">
         <v>3337872412257</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="23" t="s">
+      <c r="C75" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="D75" s="6" t="n">
+      <c r="D75" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E75" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24" t="n">
+      <c r="A76" s="25" t="n">
         <v>3337875578486</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="C76" s="23" t="s">
+      <c r="C76" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="D76" s="6" t="n">
+      <c r="D76" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E76" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="24" t="n">
+      <c r="A77" s="25" t="n">
         <v>3337872412486</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C77" s="23" t="s">
+      <c r="C77" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="D77" s="6" t="n">
+      <c r="D77" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="24" t="n">
+      <c r="A78" s="25" t="n">
         <v>3337872414091</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="C78" s="23" t="s">
+      <c r="C78" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D78" s="6" t="n">
+      <c r="D78" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="24" t="n">
+      <c r="A79" s="25" t="n">
         <v>3337872419522</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="D79" s="6" t="n">
+      <c r="D79" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="24" t="n">
+      <c r="A80" s="25" t="n">
         <v>3337872412646</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C80" s="23" t="s">
+      <c r="C80" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="D80" s="6" t="n">
+      <c r="D80" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="24" t="n">
+      <c r="A81" s="25" t="n">
         <v>3337872412264</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C81" s="23" t="s">
+      <c r="C81" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="D81" s="6" t="n">
+      <c r="D81" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E81" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="24" t="n">
+      <c r="A82" s="25" t="n">
         <v>3337872413650</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C82" s="23" t="s">
+      <c r="C82" s="24" t="s">
         <v>321</v>
       </c>
-      <c r="D82" s="6" t="n">
+      <c r="D82" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="24" t="n">
+      <c r="A83" s="25" t="n">
         <v>3337872414152</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C83" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="D83" s="6" t="n">
+      <c r="D83" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E83" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="24" t="n">
+      <c r="A84" s="25" t="n">
         <v>3337875694469</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C84" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="D84" s="6" t="n">
+      <c r="D84" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="24" t="n">
+      <c r="A85" s="25" t="n">
         <v>3337875583626</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C85" s="23" t="s">
+      <c r="C85" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="D85" s="6" t="n">
+      <c r="D85" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E85" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="24" t="n">
+      <c r="A86" s="25" t="n">
         <v>3337875683739</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C86" s="23" t="s">
+      <c r="C86" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="D86" s="6" t="n">
+      <c r="D86" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="24" t="s">
+      <c r="A87" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C87" s="23" t="s">
+      <c r="C87" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="D87" s="6" t="n">
+      <c r="D87" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="24" t="n">
+      <c r="A88" s="25" t="n">
         <v>3337875613668</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="C88" s="23" t="s">
+      <c r="C88" s="24" t="s">
         <v>334</v>
       </c>
-      <c r="D88" s="6" t="n">
+      <c r="D88" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="24" t="s">
+      <c r="A89" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C89" s="23" t="s">
+      <c r="C89" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="D89" s="6" t="n">
+      <c r="D89" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="24" t="n">
+      <c r="A90" s="25" t="n">
         <v>3337872413711</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C90" s="23" t="s">
+      <c r="C90" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="D90" s="6" t="n">
+      <c r="D90" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="24" t="n">
+      <c r="A91" s="25" t="n">
         <v>3337872413735</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="C91" s="23" t="s">
+      <c r="C91" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="D91" s="6" t="n">
+      <c r="D91" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="24" t="n">
+      <c r="A92" s="25" t="n">
         <v>3337872413728</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C92" s="23" t="s">
+      <c r="C92" s="24" t="s">
         <v>343</v>
       </c>
-      <c r="D92" s="6" t="n">
+      <c r="D92" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="24" t="s">
+      <c r="A93" s="25" t="s">
         <v>344</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C93" s="23" t="s">
+      <c r="C93" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="D93" s="6" t="n">
+      <c r="D93" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E93" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="24" t="n">
+      <c r="A94" s="25" t="n">
         <v>3337872414039</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C94" s="23" t="s">
+      <c r="C94" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="D94" s="6" t="n">
+      <c r="D94" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="24" t="n">
+      <c r="A95" s="25" t="n">
         <v>3337872412592</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C95" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="D95" s="6" t="n">
+      <c r="D95" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E95" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="24" t="n">
+      <c r="A96" s="25" t="n">
         <v>3337872413537</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="C96" s="23" t="s">
+      <c r="C96" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="D96" s="6" t="n">
+      <c r="D96" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="E96" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="24" t="n">
+      <c r="A97" s="25" t="n">
         <v>3433422404397</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C97" s="23" t="s">
+      <c r="C97" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="D97" s="6" t="n">
+      <c r="D97" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="E97" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="24" t="s">
+      <c r="A98" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C98" s="23" t="s">
+      <c r="C98" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="D98" s="6" t="n">
+      <c r="D98" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="E98" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="24" t="s">
+      <c r="A99" s="25" t="s">
         <v>358</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="C99" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="D99" s="6" t="n">
+      <c r="D99" s="7" t="n">
         <v>150</v>
       </c>
-      <c r="E99" s="6" t="s">
+      <c r="E99" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="24" t="n">
+      <c r="A100" s="25" t="n">
         <v>3337872411052</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="D100" s="6" t="n">
+      <c r="D100" s="7" t="n">
         <v>125</v>
       </c>
-      <c r="E100" s="6" t="s">
+      <c r="E100" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="51" t="n">
+      <c r="A101" s="52" t="n">
         <v>3337875685818</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C101" s="23" t="s">
+      <c r="C101" s="24" t="s">
         <v>364</v>
       </c>
-      <c r="D101" s="6" t="n">
+      <c r="D101" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E101" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="24" t="n">
+      <c r="A102" s="25" t="n">
         <v>7790033284180</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C102" s="52" t="s">
+      <c r="C102" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="D102" s="46" t="n">
+      <c r="D102" s="47" t="n">
         <v>30</v>
       </c>
-      <c r="E102" s="37" t="s">
+      <c r="E102" s="38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24" t="n">
+      <c r="A103" s="25" t="n">
         <v>3337872413667</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C103" s="53" t="s">
+      <c r="C103" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="D103" s="54" t="n">
+      <c r="D103" s="55" t="n">
         <v>40</v>
       </c>
-      <c r="E103" s="55" t="s">
+      <c r="E103" s="56" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="24" t="n">
+      <c r="A104" s="25" t="n">
         <v>7790033284173</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="C104" s="56" t="s">
+      <c r="C104" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="D104" s="57" t="n">
+      <c r="D104" s="58" t="n">
         <v>40</v>
       </c>
-      <c r="E104" s="41" t="s">
+      <c r="E104" s="42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="22" t="n">
+      <c r="A105" s="23" t="n">
         <v>3337875761031</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C105" s="35" t="s">
+      <c r="C105" s="36" t="s">
         <v>372</v>
       </c>
-      <c r="D105" s="36" t="n">
+      <c r="D105" s="37" t="n">
         <v>50</v>
       </c>
-      <c r="E105" s="58" t="s">
+      <c r="E105" s="59" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="59" t="n">
+      <c r="A106" s="60" t="n">
         <v>3337875764353</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="C106" s="39" t="s">
+      <c r="C106" s="40" t="s">
         <v>374</v>
       </c>
-      <c r="D106" s="40" t="n">
+      <c r="D106" s="41" t="n">
         <v>50</v>
       </c>
-      <c r="E106" s="60" t="s">
+      <c r="E106" s="61" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="61" t="n">
+      <c r="A107" s="62" t="n">
         <v>3337875797597</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="27" t="s">
         <v>375</v>
       </c>
-      <c r="C107" s="62" t="s">
+      <c r="C107" s="63" t="s">
         <v>376</v>
       </c>
-      <c r="D107" s="63" t="n">
+      <c r="D107" s="64" t="n">
         <v>50</v>
       </c>
-      <c r="E107" s="63" t="s">
+      <c r="E107" s="64" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="64" t="n">
+      <c r="A108" s="65" t="n">
         <v>3337875797641</v>
       </c>
-      <c r="B108" s="65" t="s">
+      <c r="B108" s="66" t="s">
         <v>377</v>
       </c>
-      <c r="C108" s="66" t="s">
+      <c r="C108" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="D108" s="67" t="n">
+      <c r="D108" s="68" t="n">
         <v>50</v>
       </c>
-      <c r="E108" s="67" t="s">
+      <c r="E108" s="68" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="64" t="n">
+      <c r="A109" s="65" t="n">
         <v>3337875797719</v>
       </c>
-      <c r="B109" s="65" t="s">
+      <c r="B109" s="66" t="s">
         <v>379</v>
       </c>
-      <c r="C109" s="68" t="s">
+      <c r="C109" s="69" t="s">
         <v>380</v>
       </c>
-      <c r="D109" s="67" t="n">
+      <c r="D109" s="68" t="n">
         <v>50</v>
       </c>
-      <c r="E109" s="67" t="s">
+      <c r="E109" s="68" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="64" t="n">
+      <c r="A110" s="65" t="n">
         <v>3337875797689</v>
       </c>
-      <c r="B110" s="65" t="s">
+      <c r="B110" s="66" t="s">
         <v>381</v>
       </c>
-      <c r="C110" s="69" t="s">
+      <c r="C110" s="70" t="s">
         <v>382</v>
       </c>
-      <c r="D110" s="67" t="n">
+      <c r="D110" s="68" t="n">
         <v>50</v>
       </c>
-      <c r="E110" s="67" t="s">
+      <c r="E110" s="68" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="64" t="n">
+      <c r="A111" s="65" t="n">
         <v>3337875797467</v>
       </c>
-      <c r="B111" s="65" t="s">
+      <c r="B111" s="66" t="s">
         <v>383</v>
       </c>
-      <c r="C111" s="68" t="s">
+      <c r="C111" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="D111" s="67" t="n">
+      <c r="D111" s="68" t="n">
         <v>50</v>
       </c>
-      <c r="E111" s="67" t="s">
+      <c r="E111" s="68" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="70" t="n">
+      <c r="A112" s="71" t="n">
         <v>3337875761123</v>
       </c>
-      <c r="B112" s="71" t="s">
+      <c r="B112" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="C112" s="72" t="s">
+      <c r="C112" s="73" t="s">
         <v>386</v>
       </c>
-      <c r="D112" s="73" t="n">
+      <c r="D112" s="74" t="n">
         <v>250</v>
       </c>
-      <c r="E112" s="73" t="s">
+      <c r="E112" s="74" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="59" t="n">
+      <c r="A113" s="60" t="n">
         <v>3337875708265</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="C113" s="74" t="s">
+      <c r="C113" s="75" t="s">
         <v>388</v>
       </c>
-      <c r="D113" s="40" t="n">
+      <c r="D113" s="41" t="n">
         <v>200</v>
       </c>
-      <c r="E113" s="60" t="s">
+      <c r="E113" s="61" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="59" t="n">
+      <c r="A114" s="60" t="n">
         <v>3337875708289</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C114" s="75" t="s">
+      <c r="C114" s="76" t="s">
         <v>390</v>
       </c>
-      <c r="D114" s="40" t="n">
+      <c r="D114" s="41" t="n">
         <v>400</v>
       </c>
-      <c r="E114" s="60" t="s">
+      <c r="E114" s="61" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="76" t="n">
+      <c r="A115" s="77" t="n">
         <v>3337875722827</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C115" s="77" t="s">
+      <c r="C115" s="78" t="s">
         <v>391</v>
       </c>
-      <c r="D115" s="78" t="n">
+      <c r="D115" s="79" t="n">
         <v>30</v>
       </c>
-      <c r="E115" s="78" t="s">
+      <c r="E115" s="79" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="79" t="n">
+      <c r="A116" s="80" t="n">
         <v>3337875729864</v>
       </c>
-      <c r="B116" s="80" t="s">
+      <c r="B116" s="81" t="s">
         <v>392</v>
       </c>
-      <c r="C116" s="81" t="s">
+      <c r="C116" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="D116" s="82" t="s">
+      <c r="D116" s="83" t="s">
         <v>394</v>
       </c>
-      <c r="E116" s="82" t="s">
+      <c r="E116" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="79" t="n">
+      <c r="A117" s="80" t="n">
         <v>3337875731409</v>
       </c>
-      <c r="B117" s="80" t="s">
+      <c r="B117" s="81" t="s">
         <v>395</v>
       </c>
-      <c r="C117" s="83" t="s">
+      <c r="C117" s="84" t="s">
         <v>396</v>
       </c>
-      <c r="D117" s="82" t="n">
+      <c r="D117" s="83" t="n">
         <v>50</v>
       </c>
-      <c r="E117" s="82" t="s">
+      <c r="E117" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="79" t="n">
+      <c r="A118" s="80" t="n">
         <v>3337875731638</v>
       </c>
-      <c r="B118" s="80" t="s">
+      <c r="B118" s="81" t="s">
         <v>397</v>
       </c>
-      <c r="C118" s="84" t="s">
+      <c r="C118" s="85" t="s">
         <v>398</v>
       </c>
-      <c r="D118" s="82" t="n">
+      <c r="D118" s="83" t="n">
         <v>50</v>
       </c>
-      <c r="E118" s="82" t="s">
+      <c r="E118" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="85" t="n">
+      <c r="A119" s="86" t="n">
         <v>3337875683739</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C119" s="82" t="s">
+      <c r="C119" s="83" t="s">
         <v>399</v>
       </c>
-      <c r="D119" s="82" t="n">
+      <c r="D119" s="83" t="n">
         <v>50</v>
       </c>
-      <c r="E119" s="82" t="s">
+      <c r="E119" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="85" t="n">
+      <c r="A120" s="86" t="n">
         <v>7790033290631</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B120" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="C120" s="82" t="s">
+      <c r="C120" s="83" t="s">
         <v>401</v>
       </c>
-      <c r="D120" s="82" t="n">
+      <c r="D120" s="83" t="n">
         <v>400</v>
       </c>
-      <c r="E120" s="82" t="s">
+      <c r="E120" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="85" t="n">
+      <c r="A121" s="86" t="n">
         <v>7790033284272</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="C121" s="86" t="s">
+      <c r="C121" s="87" t="s">
         <v>403</v>
       </c>
-      <c r="D121" s="82" t="n">
+      <c r="D121" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E121" s="82" t="s">
+      <c r="E121" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="85" t="n">
+      <c r="A122" s="86" t="n">
         <v>7790033284289</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="C122" s="86" t="s">
+      <c r="C122" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="D122" s="82" t="n">
+      <c r="D122" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E122" s="87" t="s">
+      <c r="E122" s="88" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="88" t="n">
+      <c r="A123" s="89" t="n">
         <v>3337875694469</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B123" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="C123" s="82" t="s">
+      <c r="C123" s="83" t="s">
         <v>407</v>
       </c>
-      <c r="D123" s="82" t="n">
+      <c r="D123" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E123" s="82" t="s">
+      <c r="E123" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="85" t="n">
+      <c r="A124" s="86" t="n">
         <v>7790033290624</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="C124" s="86" t="s">
+      <c r="C124" s="87" t="s">
         <v>409</v>
       </c>
-      <c r="D124" s="82" t="n">
+      <c r="D124" s="83" t="n">
         <v>40</v>
       </c>
-      <c r="E124" s="82" t="s">
+      <c r="E124" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="85" t="n">
+      <c r="A125" s="86" t="n">
         <v>3337875757515</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="C125" s="86" t="s">
+      <c r="C125" s="87" t="s">
         <v>411</v>
       </c>
-      <c r="D125" s="82" t="n">
+      <c r="D125" s="83" t="n">
         <v>20</v>
       </c>
-      <c r="E125" s="82" t="s">
+      <c r="E125" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="85" t="n">
+      <c r="A126" s="86" t="n">
         <v>3337875757614</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="C126" s="86" t="s">
+      <c r="C126" s="87" t="s">
         <v>413</v>
       </c>
-      <c r="D126" s="82" t="n">
+      <c r="D126" s="83" t="n">
         <v>40</v>
       </c>
-      <c r="E126" s="82" t="s">
+      <c r="E126" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="85" t="n">
+      <c r="A127" s="86" t="n">
         <v>3337875757669</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="C127" s="86" t="s">
+      <c r="C127" s="87" t="s">
         <v>415</v>
       </c>
-      <c r="D127" s="82" t="n">
+      <c r="D127" s="83" t="n">
         <v>40</v>
       </c>
-      <c r="E127" s="82" t="s">
+      <c r="E127" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="85" t="n">
+      <c r="A128" s="86" t="n">
         <v>7790033295384</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B128" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C128" s="86" t="s">
+      <c r="C128" s="87" t="s">
         <v>417</v>
       </c>
-      <c r="D128" s="82" t="n">
+      <c r="D128" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E128" s="82" t="s">
+      <c r="E128" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="85" t="n">
+      <c r="A129" s="86" t="n">
         <v>7790033295377</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="C129" s="86" t="s">
+      <c r="C129" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="D129" s="82" t="n">
+      <c r="D129" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E129" s="82" t="s">
+      <c r="E129" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="85" t="n">
+      <c r="A130" s="86" t="n">
         <v>7790033295360</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="C130" s="86" t="s">
+      <c r="C130" s="87" t="s">
         <v>407</v>
       </c>
-      <c r="D130" s="82" t="n">
+      <c r="D130" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E130" s="82" t="s">
+      <c r="E130" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="85" t="n">
+      <c r="A131" s="86" t="n">
         <v>7790033299665</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="C131" s="83" t="s">
+      <c r="C131" s="84" t="s">
         <v>421</v>
       </c>
-      <c r="D131" s="82" t="n">
+      <c r="D131" s="83" t="n">
         <v>30</v>
       </c>
-      <c r="E131" s="82" t="s">
+      <c r="E131" s="83" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="85" t="n">
+      <c r="A132" s="86" t="n">
         <v>7790033299672</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="C132" s="83" t="s">
+      <c r="C132" s="84" t="s">
         <v>423</v>
       </c>
-      <c r="D132" s="82" t="n">
+      <c r="D132" s="83" t="n">
         <v>40</v>
       </c>
-      <c r="E132" s="82" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="85" t="n">
-        <v>7790033299665</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="C133" s="83" t="s">
-        <v>421</v>
-      </c>
-      <c r="D133" s="82" t="n">
+      <c r="E132" s="83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A133" s="90" t="n">
+        <v>3337875890021</v>
+      </c>
+      <c r="B133" s="91" t="s">
+        <v>424</v>
+      </c>
+      <c r="C133" s="92" t="s">
+        <v>425</v>
+      </c>
+      <c r="D133" s="93" t="n">
         <v>30</v>
       </c>
-      <c r="E133" s="82" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="89" t="n">
-        <v>3337875890021</v>
-      </c>
-      <c r="B134" s="90" t="s">
-        <v>424</v>
-      </c>
-      <c r="C134" s="91" t="s">
-        <v>425</v>
-      </c>
-      <c r="D134" s="92" t="n">
-        <v>30</v>
-      </c>
-      <c r="E134" s="92" t="s">
-        <v>14</v>
-      </c>
-    </row>
+      <c r="E133" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:K133"/>
+  <autoFilter ref="A1:K132"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>